<commit_message>
Update contents of production machine
</commit_message>
<xml_diff>
--- a/imw/UT0/notes/prod_config/img/usuario_dominio.xlsx
+++ b/imw/UT0/notes/prod_config/img/usuario_dominio.xlsx
@@ -5,7 +5,7 @@
   <workbookPr checkCompatibility="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sdelquin/Dropbox/Code/claseando/imw/UT0/notes/prod_config/img/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sdelquin/Dropbox/Code/personal/claseando/imw/UT0/notes/prod_config/img/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,14 +27,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Profesor</t>
   </si>
   <si>
-    <t>Alumno</t>
-  </si>
-  <si>
     <t>sdelquin</t>
   </si>
   <si>
@@ -47,10 +44,22 @@
     <t>Dominio</t>
   </si>
   <si>
-    <t>imwpto.me</t>
-  </si>
-  <si>
     <t>aluXXXX.me</t>
+  </si>
+  <si>
+    <t>Alumnado</t>
+  </si>
+  <si>
+    <t>vps.claseando.es</t>
+  </si>
+  <si>
+    <t>Host</t>
+  </si>
+  <si>
+    <t>claseando</t>
+  </si>
+  <si>
+    <t>cloud</t>
   </si>
 </sst>
 </file>
@@ -85,7 +94,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -101,6 +110,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -132,12 +147,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -415,15 +431,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" zoomScale="320" zoomScaleNormal="320" zoomScalePageLayoutView="320" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8.5" customWidth="1"/>
+    <col min="2" max="2" width="17.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
@@ -432,29 +449,40 @@
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>2</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>7</v>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>